<commit_message>
Updated with new certificates
</commit_message>
<xml_diff>
--- a/Self Certifications.xlsx
+++ b/Self Certifications.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkansal\OneDrive - Capgemini\Prateek\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkansal\OneDrive - Capgemini\Desktop\Certificates\Certificates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="13_ncr:1_{C2E72171-ACC7-4F3D-B3EE-65CD088547A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E7D58FB9-2A53-45F5-A802-0C987794D069}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0D42AD-64E1-439A-958F-7B69DDAA20DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$135</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="158">
   <si>
     <t>Certifiction Name</t>
   </si>
@@ -246,15 +247,9 @@
     <t>IBM Applied AI</t>
   </si>
   <si>
-    <t>Python for Data Science and AI</t>
-  </si>
-  <si>
     <t>Building AI Applications with Watson APIs</t>
   </si>
   <si>
-    <t>Introduction to Computer Vision with Watson and OpenCV</t>
-  </si>
-  <si>
     <t>Applied Data Science</t>
   </si>
   <si>
@@ -484,6 +479,30 @@
   </si>
   <si>
     <t>edX</t>
+  </si>
+  <si>
+    <t>Python for Data Science, AI &amp; Development</t>
+  </si>
+  <si>
+    <t>Python Project for AI &amp; Application Development</t>
+  </si>
+  <si>
+    <t>dropped</t>
+  </si>
+  <si>
+    <t>Python Project for Data Science</t>
+  </si>
+  <si>
+    <t>Databases and SQL for Data Science with python</t>
+  </si>
+  <si>
+    <t>Data Science Fundamentals with Python and SQL</t>
+  </si>
+  <si>
+    <t>Databases and SQL for Data Science with Python</t>
+  </si>
+  <si>
+    <t>Statistics for Data Science with Python</t>
   </si>
 </sst>
 </file>
@@ -551,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -569,6 +588,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,15 +869,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E470"/>
+  <dimension ref="A1:E477"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="83.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
@@ -882,7 +900,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -936,142 +954,148 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>9</v>
+      <c r="A6" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="1">
-        <v>43997</v>
+        <v>43963</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="1">
-        <v>44024</v>
+        <v>44319</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="1">
-        <v>44059</v>
+        <v>44319</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>44323</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1">
+        <v>43975</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="1">
-        <v>43976</v>
+        <v>43997</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="1">
-        <v>44003</v>
+        <v>44024</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="1">
-        <v>44029</v>
+        <v>44059</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="1">
-        <v>44065</v>
+        <v>44319</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -1079,8 +1103,11 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B16" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>45</v>
@@ -1088,11 +1115,13 @@
       <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1">
+        <v>43976</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>26</v>
+      <c r="B17" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="C17" t="s">
         <v>45</v>
@@ -1100,11 +1129,13 @@
       <c r="D17" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>44003</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
         <v>45</v>
@@ -1112,11 +1143,13 @@
       <c r="D18" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1">
+        <v>44029</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
         <v>45</v>
@@ -1124,11 +1157,13 @@
       <c r="D19" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1">
+        <v>44065</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
         <v>45</v>
@@ -1136,14 +1171,13 @@
       <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="B21" s="4" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>45</v>
@@ -1151,13 +1185,11 @@
       <c r="D21" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="1">
-        <v>43976</v>
-      </c>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
-        <v>21</v>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>45</v>
@@ -1165,13 +1197,11 @@
       <c r="D22" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="1">
-        <v>44003</v>
-      </c>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
         <v>45</v>
@@ -1179,13 +1209,11 @@
       <c r="D23" t="s">
         <v>6</v>
       </c>
-      <c r="E23" s="1">
-        <v>44029</v>
-      </c>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
         <v>45</v>
@@ -1193,13 +1221,11 @@
       <c r="D24" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="1">
-        <v>44065</v>
-      </c>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
         <v>45</v>
@@ -1211,92 +1237,100 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="1">
-        <v>44067</v>
+        <v>43976</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="1"/>
+      <c r="E27" s="1">
+        <v>44003</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>44029</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1">
+        <v>44065</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
         <v>11</v>
       </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="1">
         <v>44067</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D32" t="s">
         <v>6</v>
@@ -1305,53 +1339,51 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
         <v>38</v>
       </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="1">
-        <v>44033</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" t="s">
-        <v>45</v>
-      </c>
       <c r="D35" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="1">
-        <v>44038</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D36" t="s">
         <v>6</v>
@@ -1359,11 +1391,11 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
-        <v>47</v>
+      <c r="B37" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D37" t="s">
         <v>6</v>
@@ -1372,84 +1404,95 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" t="s">
         <v>45</v>
       </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" t="s">
-        <v>51</v>
-      </c>
       <c r="D39" t="s">
         <v>6</v>
       </c>
       <c r="E39" s="1">
-        <v>44088</v>
+        <v>44033</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D40" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="1">
+        <v>44038</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D41" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="1"/>
+      <c r="E41" s="1">
+        <v>44320</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C42" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D42" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="1"/>
+      <c r="E42" s="1">
+        <v>44322</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1">
+        <v>44322</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
-        <v>56</v>
+      <c r="A44" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C44" t="s">
         <v>51</v>
@@ -1457,359 +1500,351 @@
       <c r="D44" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="1"/>
+      <c r="E44" s="1">
+        <v>44088</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="B45" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="1">
+      <c r="C50" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" s="1">
         <v>43967</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="3" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46" s="1">
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="1">
         <v>44000</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="4" t="s">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C47" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" t="s">
-        <v>6</v>
-      </c>
-      <c r="E47" s="1">
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="1">
         <v>44025</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="3" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="1">
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="1">
         <v>44067</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="3" t="s">
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B56" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C51" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="1">
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="1">
         <v>43996</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52" t="s">
-        <v>6</v>
-      </c>
-      <c r="E52" s="1">
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="1">
         <v>43954</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C53" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="1">
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="1">
         <v>44029</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B59" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C54" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="1">
+      <c r="C59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="1">
         <v>43996</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" s="1">
+      <c r="C60" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="1">
         <v>44020</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="3" t="s">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" s="1">
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="1">
         <v>44031</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B62" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" s="1">
+      <c r="C62" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="1">
         <v>43996</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="3" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C58" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="1">
+      <c r="C63" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="1">
         <v>44020</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="4" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C59" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59" s="1">
+      <c r="C64" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="1">
         <v>44031</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="1">
+        <v>43998</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" s="11">
+        <v>44319</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C60" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" s="1">
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" s="1">
+        <v>44069</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" s="1">
         <v>43998</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C61" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="1">
-        <v>44069</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="1">
-        <v>43998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" s="1">
-        <v>44020</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" s="1">
-        <v>44044</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66" s="1">
-        <v>44067</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67" s="1">
-        <v>43954</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C68" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68" s="1">
-        <v>43963</v>
-      </c>
-    </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
-        <v>81</v>
+      <c r="A69" s="10"/>
+      <c r="B69" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C69" t="s">
         <v>5</v>
@@ -1818,12 +1853,12 @@
         <v>6</v>
       </c>
       <c r="E69" s="1">
-        <v>43967</v>
+        <v>44319</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C70" t="s">
         <v>5</v>
@@ -1832,12 +1867,12 @@
         <v>6</v>
       </c>
       <c r="E70" s="1">
-        <v>43998</v>
+        <v>44020</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C71" t="s">
         <v>5</v>
@@ -1846,7 +1881,7 @@
         <v>6</v>
       </c>
       <c r="E71" s="1">
-        <v>43975</v>
+        <v>44044</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1860,12 +1895,15 @@
         <v>6</v>
       </c>
       <c r="E72" s="1">
-        <v>44020</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="B73" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
@@ -1874,12 +1912,12 @@
         <v>6</v>
       </c>
       <c r="E73" s="1">
-        <v>44044</v>
+        <v>43954</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C74" t="s">
         <v>5</v>
@@ -1888,12 +1926,12 @@
         <v>6</v>
       </c>
       <c r="E74" s="1">
-        <v>43967</v>
+        <v>43963</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
@@ -1902,15 +1940,12 @@
         <v>6</v>
       </c>
       <c r="E75" s="1">
-        <v>44067</v>
+        <v>43967</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="9" t="s">
-        <v>83</v>
-      </c>
       <c r="B76" s="3" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="C76" t="s">
         <v>5</v>
@@ -1919,12 +1954,12 @@
         <v>6</v>
       </c>
       <c r="E76" s="1">
-        <v>44065</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
-        <v>65</v>
+      <c r="B77" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C77" t="s">
         <v>5</v>
@@ -1933,12 +1968,12 @@
         <v>6</v>
       </c>
       <c r="E77" s="1">
-        <v>43996</v>
+        <v>44319</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
-        <v>66</v>
+      <c r="B78" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="C78" t="s">
         <v>5</v>
@@ -1947,15 +1982,12 @@
         <v>6</v>
       </c>
       <c r="E78" s="1">
-        <v>43954</v>
+        <v>43975</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>66</v>
+      <c r="B79" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C79" t="s">
         <v>5</v>
@@ -1964,12 +1996,12 @@
         <v>6</v>
       </c>
       <c r="E79" s="1">
-        <v>43954</v>
+        <v>44020</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="3" t="s">
-        <v>80</v>
+      <c r="B80" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -1978,12 +2010,12 @@
         <v>6</v>
       </c>
       <c r="E80" s="1">
-        <v>43963</v>
+        <v>44044</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
-        <v>81</v>
+      <c r="B81" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C81" t="s">
         <v>5</v>
@@ -1997,7 +2029,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C82" t="s">
         <v>5</v>
@@ -2006,194 +2038,209 @@
         <v>6</v>
       </c>
       <c r="E82" s="1">
-        <v>43975</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D83" t="s">
         <v>6</v>
       </c>
       <c r="E83" s="1">
-        <v>43971</v>
+        <v>44065</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D84" t="s">
         <v>6</v>
       </c>
       <c r="E84" s="1">
-        <v>43971</v>
+        <v>43996</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="4" t="s">
-        <v>89</v>
+      <c r="B85" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="C85" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D85" t="s">
         <v>6</v>
       </c>
       <c r="E85" s="1">
-        <v>43968</v>
+        <v>43954</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="B86" s="4" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="C86" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D86" t="s">
         <v>6</v>
       </c>
       <c r="E86" s="1">
-        <v>43992</v>
+        <v>43954</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="4" t="s">
-        <v>91</v>
+      <c r="B87" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C87" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D87" t="s">
         <v>6</v>
       </c>
       <c r="E87" s="1">
-        <v>43992</v>
+        <v>43963</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="6" t="s">
-        <v>92</v>
-      </c>
       <c r="B88" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C88" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="D88" t="s">
         <v>6</v>
       </c>
       <c r="E88" s="1">
-        <v>44028</v>
+        <v>43967</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="C89" t="s">
-        <v>94</v>
+        <v>5</v>
       </c>
       <c r="D89" t="s">
         <v>6</v>
       </c>
-      <c r="E89" s="1"/>
+      <c r="E89" s="1">
+        <v>43975</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="B90" s="4" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C90" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="D90" t="s">
         <v>6</v>
       </c>
-      <c r="E90" s="1"/>
+      <c r="E90" s="1">
+        <v>43971</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="3" t="s">
-        <v>97</v>
+      <c r="B91" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="C91" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="D91" t="s">
         <v>6</v>
       </c>
-      <c r="E91" s="1"/>
+      <c r="E91" s="1">
+        <v>43971</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="3" t="s">
-        <v>98</v>
+      <c r="B92" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="C92" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="D92" t="s">
         <v>6</v>
       </c>
-      <c r="E92" s="1"/>
+      <c r="E92" s="1">
+        <v>43968</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="7" t="s">
-        <v>99</v>
-      </c>
       <c r="B93" s="4" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C93" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="D93" t="s">
         <v>6</v>
       </c>
       <c r="E93" s="1">
-        <v>44070</v>
+        <v>43992</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C94" t="s">
-        <v>102</v>
+        <v>11</v>
       </c>
       <c r="D94" t="s">
         <v>6</v>
       </c>
-      <c r="E94" s="1"/>
+      <c r="E94" s="1">
+        <v>43992</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="3" t="s">
-        <v>103</v>
+      <c r="A95" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="C95" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D95" t="s">
         <v>6</v>
       </c>
-      <c r="E95" s="1"/>
+      <c r="E95" s="1">
+        <v>44028</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="3" t="s">
-        <v>104</v>
+      <c r="B96" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="C96" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D96" t="s">
         <v>6</v>
@@ -2201,14 +2248,11 @@
       <c r="E96" s="1"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>106</v>
+      <c r="B97" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="C97" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="D97" t="s">
         <v>6</v>
@@ -2217,10 +2261,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C98" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
       <c r="D98" t="s">
         <v>6</v>
@@ -2229,453 +2273,524 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B99" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C99" t="s">
+        <v>92</v>
+      </c>
+      <c r="D99" t="s">
+        <v>6</v>
+      </c>
+      <c r="E99" s="1"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C100" t="s">
+        <v>100</v>
+      </c>
+      <c r="D100" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" s="1">
+        <v>44070</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C101" t="s">
+        <v>100</v>
+      </c>
+      <c r="D101" t="s">
+        <v>6</v>
+      </c>
+      <c r="E101" s="1"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B102" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C102" t="s">
+        <v>100</v>
+      </c>
+      <c r="D102" t="s">
+        <v>6</v>
+      </c>
+      <c r="E102" s="1"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B103" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C103" t="s">
+        <v>100</v>
+      </c>
+      <c r="D103" t="s">
+        <v>6</v>
+      </c>
+      <c r="E103" s="1"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C104" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" t="s">
+        <v>6</v>
+      </c>
+      <c r="E104" s="1"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+      <c r="D105" t="s">
+        <v>6</v>
+      </c>
+      <c r="E105" s="1"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B106" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" t="s">
+        <v>6</v>
+      </c>
+      <c r="E106" s="1"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B107" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" t="s">
+        <v>6</v>
+      </c>
+      <c r="E107" s="1"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>111</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" t="s">
+        <v>112</v>
+      </c>
+      <c r="D108" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" s="1"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>113</v>
+      </c>
+      <c r="B109" s="3"/>
+      <c r="C109" t="s">
+        <v>114</v>
+      </c>
+      <c r="D109" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="1"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110" s="3"/>
+      <c r="C110" t="s">
+        <v>100</v>
+      </c>
+      <c r="D110" t="s">
+        <v>6</v>
+      </c>
+      <c r="E110" s="1"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" s="3"/>
+      <c r="C111" t="s">
+        <v>100</v>
+      </c>
+      <c r="D111" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111" s="1"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>117</v>
+      </c>
+      <c r="B112" s="3"/>
+      <c r="C112" t="s">
+        <v>11</v>
+      </c>
+      <c r="D112" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112" s="1"/>
+    </row>
+    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B113" s="3"/>
+      <c r="C113" t="s">
+        <v>109</v>
+      </c>
+      <c r="D113" t="s">
+        <v>6</v>
+      </c>
+      <c r="E113" s="1"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>108</v>
       </c>
-      <c r="C99" t="s">
-        <v>5</v>
-      </c>
-      <c r="D99" t="s">
-        <v>6</v>
-      </c>
-      <c r="E99" s="1"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="3" t="s">
+      <c r="B114" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C114" t="s">
         <v>109</v>
       </c>
-      <c r="C100" t="s">
-        <v>5</v>
-      </c>
-      <c r="D100" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" s="1"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>113</v>
-      </c>
-      <c r="B101" s="3"/>
-      <c r="C101" t="s">
-        <v>114</v>
-      </c>
-      <c r="D101" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="1"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>115</v>
-      </c>
-      <c r="B102" s="3"/>
-      <c r="C102" t="s">
-        <v>116</v>
-      </c>
-      <c r="D102" t="s">
-        <v>6</v>
-      </c>
-      <c r="E102" s="1"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>117</v>
-      </c>
-      <c r="B103" s="3"/>
-      <c r="C103" t="s">
-        <v>102</v>
-      </c>
-      <c r="D103" t="s">
-        <v>6</v>
-      </c>
-      <c r="E103" s="1"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>118</v>
-      </c>
-      <c r="B104" s="3"/>
-      <c r="C104" t="s">
-        <v>102</v>
-      </c>
-      <c r="D104" t="s">
-        <v>6</v>
-      </c>
-      <c r="E104" s="1"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="D114" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" s="1">
+        <v>43993</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
         <v>119</v>
       </c>
-      <c r="B105" s="3"/>
-      <c r="C105" t="s">
-        <v>11</v>
-      </c>
-      <c r="D105" t="s">
-        <v>6</v>
-      </c>
-      <c r="E105" s="1"/>
-    </row>
-    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+      <c r="C115" t="s">
         <v>120</v>
       </c>
-      <c r="B106" s="3"/>
-      <c r="C106" t="s">
-        <v>111</v>
-      </c>
-      <c r="D106" t="s">
-        <v>6</v>
-      </c>
-      <c r="E106" s="1"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>110</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C107" t="s">
-        <v>111</v>
-      </c>
-      <c r="D107" t="s">
-        <v>6</v>
-      </c>
-      <c r="E107" s="1">
-        <v>43993</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
+      <c r="D115" t="s">
+        <v>6</v>
+      </c>
+      <c r="E115" s="1"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
         <v>121</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C116" t="s">
+        <v>120</v>
+      </c>
+      <c r="D116" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" s="1"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D108" t="s">
-        <v>6</v>
-      </c>
-      <c r="E108" s="1"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
+      <c r="C117" t="s">
+        <v>120</v>
+      </c>
+      <c r="D117" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" s="1"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C109" t="s">
-        <v>122</v>
-      </c>
-      <c r="D109" t="s">
-        <v>6</v>
-      </c>
-      <c r="E109" s="1"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="3" t="s">
+      <c r="C118" t="s">
         <v>124</v>
       </c>
-      <c r="C110" t="s">
-        <v>122</v>
-      </c>
-      <c r="D110" t="s">
-        <v>6</v>
-      </c>
-      <c r="E110" s="1"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B111" s="3" t="s">
+      <c r="D118" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" s="1"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B119" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C119" t="s">
         <v>126</v>
       </c>
-      <c r="D111" t="s">
-        <v>6</v>
-      </c>
-      <c r="E111" s="1"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B112" s="3" t="s">
+      <c r="D119" t="s">
+        <v>6</v>
+      </c>
+      <c r="E119" s="1"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B120" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C120" t="s">
         <v>128</v>
       </c>
-      <c r="D112" t="s">
-        <v>6</v>
-      </c>
-      <c r="E112" s="1"/>
-    </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="3" t="s">
+      <c r="D120" t="s">
+        <v>128</v>
+      </c>
+      <c r="E120" s="1">
+        <v>42348</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B121" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C121" t="s">
+        <v>128</v>
+      </c>
+      <c r="D121" t="s">
+        <v>128</v>
+      </c>
+      <c r="E121" s="1">
+        <v>42347</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B122" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C122" t="s">
+        <v>5</v>
+      </c>
+      <c r="D122" t="s">
         <v>130</v>
       </c>
-      <c r="D113" t="s">
+      <c r="E122" s="1">
+        <v>43968</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B123" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C123" t="s">
+        <v>132</v>
+      </c>
+      <c r="D123" t="s">
         <v>130</v>
       </c>
-      <c r="E113" s="1">
-        <v>42348</v>
-      </c>
-    </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B114" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="C114" t="s">
+      <c r="E123" s="1">
+        <v>43964</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B124" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C124" t="s">
+        <v>5</v>
+      </c>
+      <c r="D124" t="s">
         <v>130</v>
       </c>
-      <c r="D114" t="s">
-        <v>130</v>
-      </c>
-      <c r="E114" s="1">
-        <v>42347</v>
-      </c>
-    </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B115" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C115" t="s">
-        <v>5</v>
-      </c>
-      <c r="D115" t="s">
-        <v>132</v>
-      </c>
-      <c r="E115" s="1">
+      <c r="E124" s="1">
         <v>43968</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B116" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C116" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B125" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D116" t="s">
-        <v>132</v>
-      </c>
-      <c r="E116" s="1">
-        <v>43964</v>
-      </c>
-    </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B117" s="3" t="s">
+      <c r="C125" t="s">
         <v>135</v>
       </c>
-      <c r="C117" t="s">
-        <v>5</v>
-      </c>
-      <c r="D117" t="s">
-        <v>132</v>
-      </c>
-      <c r="E117" s="1">
-        <v>43968</v>
-      </c>
-    </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B118" s="3" t="s">
+      <c r="D125" t="s">
+        <v>135</v>
+      </c>
+      <c r="E125" s="1">
+        <v>44089</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B126" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C126" t="s">
+        <v>135</v>
+      </c>
+      <c r="D126" t="s">
+        <v>135</v>
+      </c>
+      <c r="E126" s="1">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B127" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D118" t="s">
-        <v>137</v>
-      </c>
-      <c r="E118" s="1">
-        <v>44089</v>
-      </c>
-    </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B119" s="3" t="s">
+      <c r="C127" t="s">
+        <v>135</v>
+      </c>
+      <c r="D127" t="s">
+        <v>135</v>
+      </c>
+      <c r="E127" s="1">
+        <v>44085</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B128" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C119" t="s">
-        <v>137</v>
-      </c>
-      <c r="D119" t="s">
-        <v>137</v>
-      </c>
-      <c r="E119" s="1">
-        <v>44084</v>
-      </c>
-    </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B120" s="3" t="s">
+      <c r="C128" t="s">
         <v>139</v>
       </c>
-      <c r="C120" t="s">
-        <v>137</v>
-      </c>
-      <c r="D120" t="s">
-        <v>137</v>
-      </c>
-      <c r="E120" s="1">
-        <v>44085</v>
-      </c>
-    </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B121" s="3" t="s">
+      <c r="D128" t="s">
+        <v>139</v>
+      </c>
+      <c r="E128" s="1">
+        <v>44056</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C129" t="s">
+        <v>139</v>
+      </c>
+      <c r="D129" t="s">
+        <v>139</v>
+      </c>
+      <c r="E129" s="1">
+        <v>44056</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B130" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="D121" t="s">
-        <v>141</v>
-      </c>
-      <c r="E121" s="1">
-        <v>44056</v>
-      </c>
-    </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B122" s="3" t="s">
+      <c r="C130" t="s">
         <v>142</v>
       </c>
-      <c r="C122" t="s">
-        <v>141</v>
-      </c>
-      <c r="D122" t="s">
-        <v>141</v>
-      </c>
-      <c r="E122" s="1">
-        <v>44056</v>
-      </c>
-    </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B123" s="3" t="s">
+      <c r="D130" t="s">
+        <v>142</v>
+      </c>
+      <c r="E130" s="1">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C131" t="s">
+        <v>142</v>
+      </c>
+      <c r="D131" t="s">
+        <v>142</v>
+      </c>
+      <c r="E131" s="1">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D123" t="s">
-        <v>144</v>
-      </c>
-      <c r="E123" s="1">
+      <c r="C132" t="s">
+        <v>142</v>
+      </c>
+      <c r="D132" t="s">
+        <v>142</v>
+      </c>
+      <c r="E132" s="1">
         <v>42639</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B124" s="3" t="s">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C133" t="s">
+        <v>142</v>
+      </c>
+      <c r="D133" t="s">
+        <v>142</v>
+      </c>
+      <c r="E133" s="1">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B134" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C124" t="s">
-        <v>144</v>
-      </c>
-      <c r="D124" t="s">
-        <v>144</v>
-      </c>
-      <c r="E124" s="1">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B125" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C125" t="s">
-        <v>144</v>
-      </c>
-      <c r="D125" t="s">
-        <v>144</v>
-      </c>
-      <c r="E125" s="1">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B126" s="3" t="s">
+      <c r="C134" t="s">
+        <v>142</v>
+      </c>
+      <c r="D134" t="s">
+        <v>142</v>
+      </c>
+      <c r="E134" s="1">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B135" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C135" t="s">
         <v>148</v>
       </c>
-      <c r="C126" t="s">
-        <v>144</v>
-      </c>
-      <c r="D126" t="s">
-        <v>144</v>
-      </c>
-      <c r="E126" s="1">
-        <v>42639</v>
-      </c>
-    </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C127" t="s">
-        <v>144</v>
-      </c>
-      <c r="D127" t="s">
-        <v>144</v>
-      </c>
-      <c r="E127" s="1">
-        <v>42640</v>
-      </c>
-    </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B128" s="3" t="s">
+      <c r="D135" t="s">
         <v>149</v>
       </c>
-      <c r="C128" t="s">
-        <v>150</v>
-      </c>
-      <c r="D128" t="s">
-        <v>151</v>
-      </c>
-      <c r="E128" s="1">
+      <c r="E135" s="1">
         <v>43762</v>
       </c>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E129" s="1"/>
-    </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E130" s="1"/>
-    </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E131" s="1"/>
-    </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E132" s="1"/>
-    </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E133" s="1"/>
-    </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E134" s="1"/>
-    </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E135" s="1"/>
-    </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E136" s="1"/>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E137" s="1"/>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E138" s="1"/>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E139" s="1"/>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E140" s="1"/>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E141" s="1"/>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E142" s="1"/>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E143" s="1"/>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E144" s="1"/>
     </row>
     <row r="145" spans="5:5" x14ac:dyDescent="0.25">
@@ -3655,9 +3770,288 @@
     </row>
     <row r="470" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E470" s="1"/>
+    </row>
+    <row r="471" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E471" s="1"/>
+    </row>
+    <row r="472" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E472" s="1"/>
+    </row>
+    <row r="473" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E473" s="1"/>
+    </row>
+    <row r="474" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E474" s="1"/>
+    </row>
+    <row r="475" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E475" s="1"/>
+    </row>
+    <row r="476" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E476" s="1"/>
+    </row>
+    <row r="477" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E477" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1369B4E-E952-412D-B8C9-836ABFCBC8BE}">
+  <dimension ref="A1:A48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>